<commit_message>
Uploaded routes and added to logbook
</commit_message>
<xml_diff>
--- a/Logbook/Logbook.xlsx
+++ b/Logbook/Logbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samueldelamotte/Documents/GitHub/intrusion-ai-CANsniffer-v2/Logbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A889AEB-D619-F949-804F-C9ACB344CEA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B63B3A-AE61-1543-88B9-9431255B5793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18120" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>14.2km</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>IGA Xpress Bayswater, 81 Whatley Cres, Bayswater WA 6053</t>
   </si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>driving_style</t>
-  </si>
-  <si>
-    <t>distance</t>
   </si>
   <si>
     <t>origin</t>
@@ -72,6 +66,24 @@
   </si>
   <si>
     <t>wet</t>
+  </si>
+  <si>
+    <t>log-(16-07-2020_11-29-59)</t>
+  </si>
+  <si>
+    <t>31 Drake Street, Bayswater WA 6053</t>
+  </si>
+  <si>
+    <t>Little Petra, 18b Hood St, Subiaco WA 6008</t>
+  </si>
+  <si>
+    <t>7 Piaggio Court, Bayswater WA 6053</t>
+  </si>
+  <si>
+    <t>distance (km)</t>
+  </si>
+  <si>
+    <t>log-(16-07-2020_12-12-08)</t>
   </si>
 </sst>
 </file>
@@ -443,14 +455,14 @@
   <dimension ref="A1:M677"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="72.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
@@ -458,25 +470,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -487,44 +499,72 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3">
         <v>43981</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
+      <c r="B3" s="3">
+        <v>44028</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
+      <c r="D3" s="1">
+        <v>11.3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44028</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Completed Passive Driving Collection, Started Agrressive Driving Collection
</commit_message>
<xml_diff>
--- a/Logbook/Logbook.xlsx
+++ b/Logbook/Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samueldelamotte/Documents/GitHub/intrusion-ai-CANsniffer-v2/Logbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B63B3A-AE61-1543-88B9-9431255B5793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFF5049-A055-3C43-8D07-5432506B8771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18120" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30580" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>IGA Xpress Bayswater, 81 Whatley Cres, Bayswater WA 6053</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>log-(16-07-2020_12-12-08)</t>
+  </si>
+  <si>
+    <t>log-(29-07-2020_11-46-07)</t>
+  </si>
+  <si>
+    <t>Clarko Reserve, West Coast Drive, Trigg WA</t>
+  </si>
+  <si>
+    <t>Jubilee reserve, Robinson Road, Eden Hill WA</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Freeway</t>
+  </si>
+  <si>
+    <t>log-(29-07-2020_12-55-54)</t>
+  </si>
+  <si>
+    <t>log-(29-07-2020_14-09-34)</t>
+  </si>
+  <si>
+    <t>aggressive</t>
   </si>
 </sst>
 </file>
@@ -455,7 +485,7 @@
   <dimension ref="A1:M677"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +520,9 @@
       <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -519,6 +551,9 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -542,6 +577,9 @@
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -565,33 +603,87 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44041</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44041</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44041</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
Added 2 more aggressive driving runs
</commit_message>
<xml_diff>
--- a/Logbook/Logbook.xlsx
+++ b/Logbook/Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samueldelamotte/Documents/GitHub/intrusion-ai-CANsniffer-v2/Logbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFF5049-A055-3C43-8D07-5432506B8771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7A1269-211A-594D-8DE5-AF80C8194E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30580" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
+    <workbookView xWindow="6240" yWindow="480" windowWidth="27360" windowHeight="19700" xr2:uid="{16F54D5C-2797-0840-826E-D5409ED99889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>IGA Xpress Bayswater, 81 Whatley Cres, Bayswater WA 6053</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>aggressive</t>
+  </si>
+  <si>
+    <t>log-(31-07-2020_12-27-26)</t>
+  </si>
+  <si>
+    <t>log-(31-07-2020_12-55-39)</t>
+  </si>
+  <si>
+    <t>9A Reid St, Bassendean WA 6054</t>
   </si>
 </sst>
 </file>
@@ -485,7 +494,7 @@
   <dimension ref="A1:M677"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,22 +695,56 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44043</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44043</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>

</xml_diff>